<commit_message>
Run models with new age groups
</commit_message>
<xml_diff>
--- a/Data/Dictionary_Variables.xlsx
+++ b/Data/Dictionary_Variables.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmbus\Google Drive\Pablo\Educacion\Aprendizaje Continuo\Codigos utiles\R\Proyectos R\MortalityRR-PM2.5\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Google Drive\Pablo\Educacion\Aprendizaje Continuo\Codigos utiles\R\Proyectos R\MortalityRR-PM2.5\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7656"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="369">
   <si>
     <t>descripcion</t>
   </si>
@@ -555,9 +555,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Air pollution</t>
-  </si>
-  <si>
     <t>PM2.5 2017-2019 [ug/m3]</t>
   </si>
   <si>
@@ -615,21 +612,9 @@
     <t>Wood consumption</t>
   </si>
   <si>
-    <t>% Wood as main fuel in cooking</t>
-  </si>
-  <si>
-    <t>% Wood as main fuel in heating</t>
-  </si>
-  <si>
-    <t>% Wood as main fuel in warm water</t>
-  </si>
-  <si>
     <t>Demography</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
     <t>Commune with PDA</t>
   </si>
   <si>
@@ -669,18 +654,12 @@
     <t>Area of district zones [m2]</t>
   </si>
   <si>
-    <t xml:space="preserve">% Ethnicity Origin </t>
-  </si>
-  <si>
     <t>Mortalidad</t>
   </si>
   <si>
     <t>Mortality</t>
   </si>
   <si>
-    <t>Commune density [hab/km2]</t>
-  </si>
-  <si>
     <t>Mean population district zones [hab/km2]</t>
   </si>
   <si>
@@ -690,9 +669,6 @@
     <t>P90 population district zones [hab/km2]</t>
   </si>
   <si>
-    <t>Commune density (urban area) [hab/km2]</t>
-  </si>
-  <si>
     <t>Total deaths</t>
   </si>
   <si>
@@ -855,36 +831,6 @@
     <t>Rate of hospital beds [per 100,000]</t>
   </si>
   <si>
-    <t>HDD 15°C</t>
-  </si>
-  <si>
-    <t>HDD 15°C Fall</t>
-  </si>
-  <si>
-    <t>HDD 15°C Spring</t>
-  </si>
-  <si>
-    <t>HDD 15°C Summer</t>
-  </si>
-  <si>
-    <t>HDD 15°C Winter</t>
-  </si>
-  <si>
-    <t>HDD 18°C</t>
-  </si>
-  <si>
-    <t>HDD 18°C Fall</t>
-  </si>
-  <si>
-    <t>HDD 18°C Spring</t>
-  </si>
-  <si>
-    <t>HDD 18°C Summer</t>
-  </si>
-  <si>
-    <t>HDD 18°C Winter</t>
-  </si>
-  <si>
     <t>Average relative humidity [%]</t>
   </si>
   <si>
@@ -936,9 +882,6 @@
     <t>Mortality rate Cardiovascular (all I) [per 100,000]</t>
   </si>
   <si>
-    <t>Medium overcrowding in housing [2.5 to 5 hab. per room]</t>
-  </si>
-  <si>
     <t>Indice de hacinamiento medio [2.5 a 5 personas por dormitorio]</t>
   </si>
   <si>
@@ -975,12 +918,6 @@
     <t>perc_overcrowding_high</t>
   </si>
   <si>
-    <t>Low overcrowding in housing [less than 2.5 hab. per room]</t>
-  </si>
-  <si>
-    <t>High overcrowding in housing [more than 5 hab. per room]</t>
-  </si>
-  <si>
     <t>Indice de hacinamiento bajo [menos de 2.5 personas por dormitorio]</t>
   </si>
   <si>
@@ -1101,9 +1038,6 @@
     <t>perc_wood_avg</t>
   </si>
   <si>
-    <t>% Wood as main fuel</t>
-  </si>
-  <si>
     <t>mrAdj_LCA</t>
   </si>
   <si>
@@ -1132,6 +1066,66 @@
   </si>
   <si>
     <t>Adjusted mortality rate Lung Cancer (C33-C34) [per 100,000]</t>
+  </si>
+  <si>
+    <t>Air pollution exposure</t>
+  </si>
+  <si>
+    <t>Population 2017</t>
+  </si>
+  <si>
+    <t>Population commune density [hab/km2]</t>
+  </si>
+  <si>
+    <t>Population commune density (urban area) [hab/km2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Native Origin </t>
+  </si>
+  <si>
+    <t>% Low overcrowding in housing [less than 2.5 hab. per room]</t>
+  </si>
+  <si>
+    <t>% Medium overcrowding in housing [2.5 to 5 hab. per room]</t>
+  </si>
+  <si>
+    <t>% High overcrowding in housing [more than 5 hab. per room]</t>
+  </si>
+  <si>
+    <t>HDD 15°C Fall [°C]</t>
+  </si>
+  <si>
+    <t>HDD 15°C Spring [°C]</t>
+  </si>
+  <si>
+    <t>HDD 15°C Summer [°C]</t>
+  </si>
+  <si>
+    <t>HDD 15°C Winter [°C]</t>
+  </si>
+  <si>
+    <t>HDD 18°C Fall [°C]</t>
+  </si>
+  <si>
+    <t>HDD 18°C Spring [°C]</t>
+  </si>
+  <si>
+    <t>HDD 18°C Summer [°C]</t>
+  </si>
+  <si>
+    <t>HDD 18°C Winter [°C]</t>
+  </si>
+  <si>
+    <t>% Wood usage as main fuel in cooking</t>
+  </si>
+  <si>
+    <t>% Wood usage as main fuel in heating</t>
+  </si>
+  <si>
+    <t>% Wood usage as main fuel in warm water</t>
+  </si>
+  <si>
+    <t>% Wood usage as main fuel</t>
   </si>
 </sst>
 </file>
@@ -1941,19 +1935,19 @@
   <dimension ref="A1:E136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="68.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1970,768 +1964,768 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B3" t="s">
         <v>349</v>
-      </c>
-      <c r="B3" t="s">
-        <v>178</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>349</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
         <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>198</v>
+        <v>365</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="B24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>199</v>
+        <v>366</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>200</v>
+        <v>367</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
       </c>
       <c r="D27" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="B28" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
         <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>202</v>
+        <v>350</v>
       </c>
       <c r="E28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="E29" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
         <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="B31" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C31" t="s">
         <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C32" t="s">
         <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C33" t="s">
         <v>45</v>
       </c>
       <c r="D33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E33" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C34" t="s">
         <v>45</v>
       </c>
       <c r="D34" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
         <v>45</v>
       </c>
       <c r="D35" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D36" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C37" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D37" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D38" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="B39" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C39" t="s">
         <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="B40" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C41" t="s">
         <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C42" t="s">
         <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>219</v>
+        <v>351</v>
       </c>
       <c r="E42" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="B43" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C43" t="s">
         <v>45</v>
       </c>
       <c r="D43" t="s">
-        <v>223</v>
+        <v>352</v>
       </c>
       <c r="E43" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="B44" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
       </c>
       <c r="D44" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="E44" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="B45" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C45" t="s">
         <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>216</v>
+        <v>353</v>
       </c>
       <c r="E45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="B46" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C46" t="s">
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="E46" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C47" t="s">
         <v>45</v>
@@ -2743,1475 +2737,1475 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C48" t="s">
         <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>318</v>
+        <v>354</v>
       </c>
       <c r="E48" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C49" t="s">
         <v>45</v>
       </c>
       <c r="D49" t="s">
-        <v>305</v>
+        <v>355</v>
       </c>
       <c r="E49" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="B50" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C50" t="s">
         <v>45</v>
       </c>
       <c r="D50" t="s">
-        <v>319</v>
+        <v>356</v>
       </c>
       <c r="E50" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C51" t="s">
+        <v>211</v>
+      </c>
+      <c r="D51" t="s">
         <v>217</v>
-      </c>
-      <c r="D51" t="s">
-        <v>225</v>
       </c>
       <c r="E51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>68</v>
       </c>
       <c r="B52" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C52" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D52" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E52" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>69</v>
       </c>
       <c r="B53" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" t="s">
+        <v>211</v>
+      </c>
+      <c r="D53" t="s">
         <v>218</v>
-      </c>
-      <c r="C53" t="s">
-        <v>217</v>
-      </c>
-      <c r="D53" t="s">
-        <v>226</v>
       </c>
       <c r="E53" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D54" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E54" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>71</v>
       </c>
       <c r="B55" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C55" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D55" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E55" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>73</v>
       </c>
       <c r="B56" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C56" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D56" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E56" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>74</v>
       </c>
       <c r="B57" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D57" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E57" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>75</v>
       </c>
       <c r="B58" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C58" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D58" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E58" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C59" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D59" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E59" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C60" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D60" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E60" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C61" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D61" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E61" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
       <c r="B62" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C62" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E62" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>80</v>
       </c>
       <c r="B63" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C63" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D63" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E63" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>81</v>
       </c>
       <c r="B64" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C64" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D64" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C65" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D65" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E65" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>83</v>
       </c>
       <c r="B66" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C66" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D66" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E66" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C67" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D67" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E67" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C68" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D68" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E68" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C69" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D69" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E69" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C70" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D70" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E70" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>89</v>
       </c>
       <c r="B71" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C71" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D71" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E71" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C72" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D72" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E72" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C73" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D73" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E73" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>93</v>
       </c>
       <c r="B74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C74" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D74" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E74" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>94</v>
       </c>
       <c r="B75" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C75" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E75" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>96</v>
       </c>
       <c r="B76" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C76" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D76" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E76" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>97</v>
       </c>
       <c r="B77" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C77" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D77" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E77" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>98</v>
       </c>
       <c r="B78" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C78" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D78" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="E78" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>99</v>
       </c>
       <c r="B79" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C79" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D79" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E79" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="B80" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C80" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D80" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D81" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B82" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C82" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D82" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="B83" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C83" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D83" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="B84" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C84" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D84" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>320</v>
+      </c>
+      <c r="B85" t="s">
+        <v>212</v>
+      </c>
+      <c r="C85" t="s">
+        <v>211</v>
+      </c>
+      <c r="D85" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>321</v>
+      </c>
+      <c r="B86" t="s">
+        <v>212</v>
+      </c>
+      <c r="C86" t="s">
+        <v>211</v>
+      </c>
+      <c r="D86" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>322</v>
+      </c>
+      <c r="B87" t="s">
+        <v>212</v>
+      </c>
+      <c r="C87" t="s">
+        <v>211</v>
+      </c>
+      <c r="D87" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>323</v>
+      </c>
+      <c r="B88" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" t="s">
+        <v>211</v>
+      </c>
+      <c r="D88" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>324</v>
+      </c>
+      <c r="B89" t="s">
+        <v>212</v>
+      </c>
+      <c r="C89" t="s">
+        <v>211</v>
+      </c>
+      <c r="D89" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>339</v>
+      </c>
+      <c r="B90" t="s">
+        <v>212</v>
+      </c>
+      <c r="C90" t="s">
+        <v>211</v>
+      </c>
+      <c r="D90" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>340</v>
+      </c>
+      <c r="B91" t="s">
+        <v>212</v>
+      </c>
+      <c r="C91" t="s">
+        <v>211</v>
+      </c>
+      <c r="D91" t="s">
         <v>341</v>
       </c>
-      <c r="B85" t="s">
-        <v>218</v>
-      </c>
-      <c r="C85" t="s">
-        <v>217</v>
-      </c>
-      <c r="D85" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>342</v>
-      </c>
-      <c r="B86" t="s">
-        <v>218</v>
-      </c>
-      <c r="C86" t="s">
-        <v>217</v>
-      </c>
-      <c r="D86" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>343</v>
-      </c>
-      <c r="B87" t="s">
-        <v>218</v>
-      </c>
-      <c r="C87" t="s">
-        <v>217</v>
-      </c>
-      <c r="D87" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>344</v>
-      </c>
-      <c r="B88" t="s">
-        <v>218</v>
-      </c>
-      <c r="C88" t="s">
-        <v>217</v>
-      </c>
-      <c r="D88" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>345</v>
-      </c>
-      <c r="B89" t="s">
-        <v>218</v>
-      </c>
-      <c r="C89" t="s">
-        <v>217</v>
-      </c>
-      <c r="D89" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>361</v>
-      </c>
-      <c r="B90" t="s">
-        <v>218</v>
-      </c>
-      <c r="C90" t="s">
-        <v>217</v>
-      </c>
-      <c r="D90" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>362</v>
-      </c>
-      <c r="B91" t="s">
-        <v>218</v>
-      </c>
-      <c r="C91" t="s">
-        <v>217</v>
-      </c>
-      <c r="D91" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="B92" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C92" t="s">
         <v>102</v>
       </c>
       <c r="D92" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E92" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>122</v>
       </c>
       <c r="B93" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C93" t="s">
         <v>102</v>
       </c>
       <c r="D93" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E93" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="B94" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C94" t="s">
         <v>102</v>
       </c>
       <c r="D94" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="E94" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="B95" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C95" t="s">
         <v>102</v>
       </c>
       <c r="D95" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E95" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="B96" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C96" t="s">
         <v>102</v>
       </c>
       <c r="D96" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E96" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="B97" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C97" t="s">
         <v>102</v>
       </c>
       <c r="D97" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E97" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>109</v>
       </c>
       <c r="B98" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C98" t="s">
         <v>102</v>
       </c>
       <c r="D98" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="E98" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>111</v>
       </c>
       <c r="B99" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C99" t="s">
         <v>102</v>
       </c>
       <c r="D99" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="E99" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>113</v>
       </c>
       <c r="B100" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C100" t="s">
         <v>102</v>
       </c>
       <c r="D100" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E100" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>115</v>
       </c>
       <c r="B101" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C101" t="s">
         <v>102</v>
       </c>
       <c r="D101" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="E101" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>117</v>
       </c>
       <c r="B102" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C102" t="s">
         <v>102</v>
       </c>
       <c r="D102" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="E102" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="B103" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C103" t="s">
         <v>102</v>
       </c>
       <c r="D103" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
       <c r="E103" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="B104" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C104" t="s">
         <v>102</v>
       </c>
       <c r="D104" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="E104" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>119</v>
       </c>
       <c r="B105" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C105" t="s">
         <v>102</v>
       </c>
       <c r="D105" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="E105" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="B106" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C106" t="s">
         <v>102</v>
       </c>
       <c r="D106" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="E106" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>125</v>
       </c>
       <c r="B107" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C107" t="s">
         <v>123</v>
       </c>
       <c r="D107" t="s">
-        <v>278</v>
+        <v>124</v>
       </c>
       <c r="E107" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>127</v>
       </c>
       <c r="B108" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C108" t="s">
         <v>123</v>
       </c>
       <c r="D108" t="s">
-        <v>279</v>
+        <v>357</v>
       </c>
       <c r="E108" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>129</v>
       </c>
       <c r="B109" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C109" t="s">
         <v>123</v>
       </c>
       <c r="D109" t="s">
-        <v>280</v>
+        <v>358</v>
       </c>
       <c r="E109" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>131</v>
       </c>
       <c r="B110" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C110" t="s">
         <v>123</v>
       </c>
       <c r="D110" t="s">
-        <v>281</v>
+        <v>359</v>
       </c>
       <c r="E110" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>133</v>
       </c>
       <c r="B111" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C111" t="s">
         <v>123</v>
       </c>
       <c r="D111" t="s">
-        <v>282</v>
+        <v>360</v>
       </c>
       <c r="E111" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>135</v>
       </c>
       <c r="B112" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C112" t="s">
         <v>123</v>
       </c>
       <c r="D112" t="s">
-        <v>283</v>
+        <v>134</v>
       </c>
       <c r="E112" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>137</v>
       </c>
       <c r="B113" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C113" t="s">
         <v>123</v>
       </c>
       <c r="D113" t="s">
-        <v>284</v>
+        <v>361</v>
       </c>
       <c r="E113" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>139</v>
       </c>
       <c r="B114" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C114" t="s">
         <v>123</v>
       </c>
       <c r="D114" t="s">
-        <v>285</v>
+        <v>362</v>
       </c>
       <c r="E114" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>141</v>
       </c>
       <c r="B115" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C115" t="s">
         <v>123</v>
       </c>
       <c r="D115" t="s">
-        <v>286</v>
+        <v>363</v>
       </c>
       <c r="E115" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>143</v>
       </c>
       <c r="B116" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C116" t="s">
         <v>123</v>
       </c>
       <c r="D116" t="s">
-        <v>287</v>
+        <v>364</v>
       </c>
       <c r="E116" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>145</v>
       </c>
       <c r="B117" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C117" t="s">
         <v>123</v>
       </c>
       <c r="D117" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="E117" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>147</v>
       </c>
       <c r="B118" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C118" t="s">
         <v>123</v>
       </c>
       <c r="D118" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="E118" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>149</v>
       </c>
       <c r="B119" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C119" t="s">
         <v>123</v>
       </c>
       <c r="D119" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="E119" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>151</v>
       </c>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C120" t="s">
         <v>123</v>
       </c>
       <c r="D120" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="E120" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>153</v>
       </c>
       <c r="B121" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C121" t="s">
         <v>123</v>
       </c>
       <c r="D121" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="E121" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>155</v>
       </c>
       <c r="B122" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C122" t="s">
         <v>123</v>
       </c>
       <c r="D122" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="E122" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>157</v>
       </c>
       <c r="B123" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C123" t="s">
         <v>123</v>
       </c>
       <c r="D123" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="E123" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>159</v>
       </c>
       <c r="B124" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C124" t="s">
         <v>123</v>
       </c>
       <c r="D124" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="E124" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>161</v>
       </c>
       <c r="B125" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C125" t="s">
         <v>123</v>
       </c>
       <c r="D125" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="E125" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>163</v>
       </c>
       <c r="B126" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C126" t="s">
         <v>123</v>
       </c>
       <c r="D126" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="E126" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>164</v>
       </c>
       <c r="B127" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C127" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D127" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E127" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>165</v>
       </c>
       <c r="B128" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C128" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D128" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="E128" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>166</v>
       </c>
       <c r="B129" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C129" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D129" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E129" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>167</v>
       </c>
       <c r="B130" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C130" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D130" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E130" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>168</v>
       </c>
       <c r="B131" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C131" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D131" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E131" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>169</v>
       </c>
       <c r="B132" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C132" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D132" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E132" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>170</v>
       </c>
       <c r="B133" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C133" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D133" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="E133" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>173</v>
       </c>
       <c r="B134" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C134" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D134" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E134" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>171</v>
       </c>
       <c r="B135" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C135" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D135" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E135" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>172</v>
       </c>
       <c r="B136" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C136" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D136" t="s">
         <v>172</v>

</xml_diff>